<commit_message>
Updated Functionality in Add Category
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AddCategory.data.xlsx
+++ b/tests/artifact/data/UI-AddCategory.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="239">
   <si>
     <t>login.screen</t>
   </si>
@@ -746,6 +746,12 @@
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div/div[2]/form/table[2]/tbody/tr[4]/td[2]/div/input</t>
+  </si>
+  <si>
+    <t>add.deleteSelection</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table[2]/tbody/tr[4]/td[2]/div/div/button[text()=' Clear Selection ']</t>
   </si>
 </sst>
 </file>
@@ -1860,10 +1866,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2837,6 +2843,14 @@
         <v>236</v>
       </c>
     </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
Updated the Add Category Script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AddCategory.data.xlsx
+++ b/tests/artifact/data/UI-AddCategory.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="288">
   <si>
     <t>login.screen</t>
   </si>
@@ -172,13 +172,13 @@
     <t>success.message</t>
   </si>
   <si>
-    <t>//*[text()='Login Success!']</t>
+    <t>//div[@class='toast-body'][contains(text(),'Login Success!']</t>
   </si>
   <si>
     <t>title.header</t>
   </si>
   <si>
-    <t>//*[text()='Welcome Accion!']</t>
+    <t>//div[@class='toast-body'][contains(text(),'Welcome Accion']</t>
   </si>
   <si>
     <t>org.open</t>
@@ -415,7 +415,7 @@
     <t>//main[@class='mb-5']/section/div/input</t>
   </si>
   <si>
-    <t>addCategory.DownloadIcon</t>
+    <t>ac.DownloadIcon</t>
   </si>
   <si>
     <t>//main[@class='mb-5']/section/section/div[3]/button</t>
@@ -577,7 +577,7 @@
     <t>/td[2]</t>
   </si>
   <si>
-    <t>table.addDelete.values</t>
+    <t>table.rate.values</t>
   </si>
   <si>
     <t>/td[3]</t>
@@ -643,13 +643,43 @@
     <t>//main[@class='mb-5']/section/div/div[2]/form/table[2]/tbody/tr[4]/td[4]/div/button[2]</t>
   </si>
   <si>
-    <t>select.Specification</t>
+    <t>select.Specification.row.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table[1]/tbody/tr</t>
+  </si>
+  <si>
+    <t>select.Specification.first</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[1]/td[1]/select</t>
+  </si>
+  <si>
+    <t>select.spec.num.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[2]/td/select</t>
+  </si>
+  <si>
+    <t>select.spec.num1.values</t>
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[3]/td/select</t>
   </si>
   <si>
-    <t>Enter.Title.Specification</t>
+    <t>Enter.Titleone.Spec.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[1]/td[2]/input</t>
+  </si>
+  <si>
+    <t>Enter.Titletwo.Spec.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[2]/td[2]/input</t>
+  </si>
+  <si>
+    <t>Enter.Titlethree.Spec.values</t>
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[3]/td[2]/input</t>
@@ -700,6 +730,21 @@
     <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[3]/td[3]/div/button[2]</t>
   </si>
   <si>
+    <t>ec.delete.spec.row.xpath</t>
+  </si>
+  <si>
+    <t>ec.delete.spec.tax.button</t>
+  </si>
+  <si>
+    <t>/td/div/button[2]</t>
+  </si>
+  <si>
+    <t>ec.delete.tax.row.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table[2]/tbody/tr</t>
+  </si>
+  <si>
     <t>save.button.AddCategory</t>
   </si>
   <si>
@@ -709,15 +754,9 @@
     <t>add.new.Specification</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[1]/td[1]/select</t>
-  </si>
-  <si>
     <t>add.new.Title</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[1]/td[2]/input</t>
-  </si>
-  <si>
     <t>add.Tax.IGST</t>
   </si>
   <si>
@@ -752,6 +791,114 @@
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div/div[2]/form/table[2]/tbody/tr[4]/td[2]/div/div/button[text()=' Clear Selection ']</t>
+  </si>
+  <si>
+    <t>values.Specification</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>values.SpecTitle</t>
+  </si>
+  <si>
+    <t>C[NUMBER(${num})=&gt;randomDigits(1)]</t>
+  </si>
+  <si>
+    <t>click.add.specification</t>
+  </si>
+  <si>
+    <t>/td[3]/div/button[1]</t>
+  </si>
+  <si>
+    <t>Specification.option.selection</t>
+  </si>
+  <si>
+    <t>/select</t>
+  </si>
+  <si>
+    <t>spec.title.value</t>
+  </si>
+  <si>
+    <t>/input</t>
+  </si>
+  <si>
+    <t>Tax.table.row.xpath</t>
+  </si>
+  <si>
+    <t>tax.state.values</t>
+  </si>
+  <si>
+    <t>/div/input</t>
+  </si>
+  <si>
+    <t>Addcategory.save.Button</t>
+  </si>
+  <si>
+    <t>addcategory.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Category ${Categoryname} created!')]</t>
+  </si>
+  <si>
+    <t>category.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Category ${addCategoryname} created!')]</t>
+  </si>
+  <si>
+    <t>editCategory.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Category ${Categoryname} Updated!')]</t>
+  </si>
+  <si>
+    <t>ac.duplicateEntry.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Duplicate Category not allowed')]</t>
+  </si>
+  <si>
+    <t>ac.list.table.delete</t>
+  </si>
+  <si>
+    <t>/td[3]/div/button</t>
+  </si>
+  <si>
+    <t>Popup.Table.name</t>
+  </si>
+  <si>
+    <t>//*[@class='modal-content']/div</t>
+  </si>
+  <si>
+    <t>click.cancel.button</t>
+  </si>
+  <si>
+    <t>//*[@class='modal-content']/footer/button[1]</t>
+  </si>
+  <si>
+    <t>click.ok.button</t>
+  </si>
+  <si>
+    <t>//*[@class='modal-content']/footer/button[2]</t>
+  </si>
+  <si>
+    <t>delete.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Category "${Categoryname}" was successfully deleted!')]</t>
+  </si>
+  <si>
+    <t>tax.add.delete.button</t>
+  </si>
+  <si>
+    <t>/td[4]/div/button[1]</t>
+  </si>
+  <si>
+    <t>spec.add.delete.button</t>
+  </si>
+  <si>
+    <t>/td[3]/div/button[2]</t>
   </si>
 </sst>
 </file>
@@ -1866,10 +2013,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2728,79 +2875,79 @@
         <v>210</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2824,31 +2971,247 @@
         <v>231</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B121" s="2" t="s">
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1" t="s">
         <v>238</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Add category and TrnasferNote script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AddCategory.data.xlsx
+++ b/tests/artifact/data/UI-AddCategory.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="300">
   <si>
     <t>login.screen</t>
   </si>
@@ -499,6 +499,12 @@
     <t>//main[@class='mb-5']/section/div/div[2]/form/fieldset[2]/div/div/select</t>
   </si>
   <si>
+    <t>parentCategory.enter.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/fieldset[2]/div/div/select/option[3]</t>
+  </si>
+  <si>
     <t>addSpecifiction.switchbox</t>
   </si>
   <si>
@@ -899,6 +905,36 @@
   </si>
   <si>
     <t>/td[3]/div/button[2]</t>
+  </si>
+  <si>
+    <t>popup.message.xpath</t>
+  </si>
+  <si>
+    <t>//div[@class='b-toaster-slot vue-portal-target']/div/div/div</t>
+  </si>
+  <si>
+    <t>specification.title.values.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table[1]/tbody/tr/td[2]</t>
+  </si>
+  <si>
+    <t>specification.button.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table[1]/tbody/tr/td[3]</t>
+  </si>
+  <si>
+    <t>delete.specification.button</t>
+  </si>
+  <si>
+    <t>/div/button[2]</t>
+  </si>
+  <si>
+    <t>Selection.field</t>
+  </si>
+  <si>
+    <t>/div/button[2]//div2</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2049,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2915,15 +2951,15 @@
         <v>220</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2939,23 +2975,23 @@
         <v>225</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2971,15 +3007,15 @@
         <v>231</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3003,23 +3039,23 @@
         <v>238</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3107,15 +3143,15 @@
         <v>262</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -3123,15 +3159,15 @@
         <v>265</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>267</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -3212,6 +3248,54 @@
       </c>
       <c r="B148" s="2" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3334,7 +3418,7 @@
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E60 B61:E1048576 B30:B40 B42:B60">
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E60 B61:E1048576 B42:B60 B30:B40">
     <cfRule type="expression" dxfId="5" priority="63" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
Worked on the review comments and Updated the script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AddCategory.data.xlsx
+++ b/tests/artifact/data/UI-AddCategory.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="313">
   <si>
     <t>login.screen</t>
   </si>
@@ -802,15 +802,39 @@
     <t>values.Specification</t>
   </si>
   <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>values.spec.Num</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
+    <t>values.spec.Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>values.SpecTitle</t>
   </si>
   <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>values.specTitle.Num</t>
+  </si>
+  <si>
     <t>C[NUMBER(${num})=&gt;randomDigits(1)]</t>
   </si>
   <si>
+    <t>values.specTitle.Date</t>
+  </si>
+  <si>
+    <t>08-01-2024</t>
+  </si>
+  <si>
     <t>click.add.specification</t>
   </si>
   <si>
@@ -935,6 +959,21 @@
   </si>
   <si>
     <t>/div/button[2]//div2</t>
+  </si>
+  <si>
+    <t>Edit.Specification.row.xpath</t>
+  </si>
+  <si>
+    <t>delete.spec.updated</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/form/table/tbody/tr[1]/td[3]/div/button[2]</t>
+  </si>
+  <si>
+    <t>spec.date.xpath.values</t>
+  </si>
+  <si>
+    <t>/html[1]/body[1]/div[1]/main[1]/section[1]/div[1]/div[2]/form[1]/table[1]/tbody[1]/tr[1]/td[2]</t>
   </si>
 </sst>
 </file>
@@ -2049,10 +2088,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -3151,55 +3190,55 @@
         <v>264</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>275</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -3296,6 +3335,62 @@
       </c>
       <c r="B154" s="2" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3418,7 +3513,7 @@
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E60 B61:E1048576 B42:B60 B30:B40">
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E1048576 B42:B133 B135:B1048576 B30:B40">
     <cfRule type="expression" dxfId="5" priority="63" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added UI Automation script for Add Category
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AddCategory.data.xlsx
+++ b/tests/artifact/data/UI-AddCategory.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="315">
   <si>
     <t>login.screen</t>
   </si>
@@ -160,7 +160,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:fb6542416f0f8d75513db5fd223b48100aefb8829d208c2a</t>
+    <t>crypt:b5ab6d48b9b42058bf7c4c38abff9836ab04ed5622fef366</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -208,7 +208,8 @@
     <t>org.Inventory</t>
   </si>
   <si>
-    <t>//*[text()='Inventory']</t>
+    <t xml:space="preserve">//div[@class='b-sidebar-body']/ul/h6/span[text()='Inventory']
+</t>
   </si>
   <si>
     <t>org.Invoice</t>
@@ -974,6 +975,12 @@
   </si>
   <si>
     <t>/html[1]/body[1]/div[1]/main[1]/section[1]/div[1]/div[2]/form[1]/table[1]/tbody[1]/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>Category.select.State</t>
+  </si>
+  <si>
+    <t>Delhi</t>
   </si>
 </sst>
 </file>
@@ -2088,10 +2095,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -3393,6 +3400,14 @@
         <v>312</v>
       </c>
     </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>